<commit_message>
Update dBu meter calculation.xlsx
</commit_message>
<xml_diff>
--- a/dBu meter calculation.xlsx
+++ b/dBu meter calculation.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Documents\GitHub\DMH-Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6889A2DB-296C-4952-A776-3CA66495079B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E4304B-DD82-42CB-9F4B-034D0DB18BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{34920A5C-097A-4EEA-8361-CAFEEE971C72}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="11v75" sheetId="2" r:id="rId1"/>
+    <sheet name="10V" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
   <si>
     <t>dBu</t>
   </si>
@@ -61,9 +62,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +76,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -100,10 +109,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,11 +447,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D0D715C-B6A8-4B52-83D1-951A7478EB04}">
-  <dimension ref="G4:L16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62D02EB-515C-4A0B-BB92-62D83B04599D}">
+  <dimension ref="G4:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,8 +473,7 @@
         <v>11.75</v>
       </c>
       <c r="J5">
-        <f>SUM(J6:J15)</f>
-        <v>174.47</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="7:12" x14ac:dyDescent="0.3">
@@ -477,17 +486,12 @@
       <c r="I6" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="2">
-        <v>68</v>
-      </c>
-      <c r="K6" s="1">
-        <f>J6/$J$5</f>
-        <v>0.38975181979709977</v>
-      </c>
-      <c r="L6" s="1">
-        <f>K6*$I$5</f>
-        <v>4.5795838826159221</v>
-      </c>
+      <c r="J6" s="3">
+        <f>J5-SUM(J7:J15)</f>
+        <v>81.349999999999994</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
     </row>
     <row r="7" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G7">
@@ -502,15 +506,15 @@
         <v>0.18600000000000003</v>
       </c>
       <c r="J7" s="2">
-        <v>32.4</v>
+        <v>5.49</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" ref="K7:K15" si="1">J7/$J$5</f>
-        <v>0.18570527884450047</v>
+        <f>SUM(J7:J15)/J5</f>
+        <v>0.1865</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7:L16" si="2">K7*$I$5</f>
-        <v>2.1820370264228806</v>
+        <f t="shared" ref="L7:L15" si="1">K7*$I$5</f>
+        <v>2.1913749999999999</v>
       </c>
     </row>
     <row r="8" spans="7:12" x14ac:dyDescent="0.3">
@@ -526,15 +530,15 @@
         <v>0.13170212765957448</v>
       </c>
       <c r="J8" s="2">
-        <v>23.3</v>
+        <v>3.83</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="1"/>
-        <v>0.1335473147245945</v>
+        <f>SUM(J8:J15)/J5</f>
+        <v>0.13160000000000002</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="2"/>
-        <v>1.5691809480139853</v>
+        <f t="shared" si="1"/>
+        <v>1.5463000000000002</v>
       </c>
     </row>
     <row r="9" spans="7:12" x14ac:dyDescent="0.3">
@@ -550,15 +554,15 @@
         <v>9.3191489361702129E-2</v>
       </c>
       <c r="J9" s="2">
-        <v>16.2</v>
+        <v>2.74</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="1"/>
-        <v>9.2852639422250235E-2</v>
+        <f>SUM(J9:J15)/J5</f>
+        <v>9.3299999999999994E-2</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="2"/>
-        <v>1.0910185132114403</v>
+        <f t="shared" si="1"/>
+        <v>1.0962749999999999</v>
       </c>
     </row>
     <row r="10" spans="7:12" x14ac:dyDescent="0.3">
@@ -574,15 +578,15 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="J10" s="2">
-        <v>11.5</v>
+        <v>1.91</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="1"/>
-        <v>6.5913910700980113E-2</v>
+        <f>SUM(J10:J15)/J5</f>
+        <v>6.5899999999999986E-2</v>
       </c>
       <c r="L10" s="1">
-        <f t="shared" si="2"/>
-        <v>0.77448845073651629</v>
+        <f t="shared" si="1"/>
+        <v>0.77432499999999982</v>
       </c>
     </row>
     <row r="11" spans="7:12" x14ac:dyDescent="0.3">
@@ -598,15 +602,15 @@
         <v>4.6723404255319151E-2</v>
       </c>
       <c r="J11" s="2">
-        <v>8.1999999999999993</v>
+        <v>1.37</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="1"/>
-        <v>4.6999484152003203E-2</v>
+        <f>SUM(J11:J15)/J5</f>
+        <v>4.6799999999999994E-2</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" si="2"/>
-        <v>0.55224393878603761</v>
+        <f t="shared" si="1"/>
+        <v>0.54989999999999994</v>
       </c>
     </row>
     <row r="12" spans="7:12" x14ac:dyDescent="0.3">
@@ -622,15 +626,15 @@
         <v>3.3063829787234045E-2</v>
       </c>
       <c r="J12" s="2">
-        <v>5.76</v>
+        <v>0.98</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="1"/>
-        <v>3.3014271794577867E-2</v>
+        <f>SUM(J12:J15)/J5</f>
+        <v>3.3099999999999997E-2</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" si="2"/>
-        <v>0.38791769358628991</v>
+        <f t="shared" si="1"/>
+        <v>0.38892499999999997</v>
       </c>
     </row>
     <row r="13" spans="7:12" x14ac:dyDescent="0.3">
@@ -646,15 +650,15 @@
         <v>2.3404255319148939E-2</v>
       </c>
       <c r="J13" s="2">
-        <v>4.12</v>
+        <v>0.68</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="1"/>
-        <v>2.3614374964177225E-2</v>
+        <f>SUM(J13:J15)/J5</f>
+        <v>2.3300000000000001E-2</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="2"/>
-        <v>0.2774689058290824</v>
+        <f t="shared" si="1"/>
+        <v>0.27377499999999999</v>
       </c>
     </row>
     <row r="14" spans="7:12" x14ac:dyDescent="0.3">
@@ -670,15 +674,15 @@
         <v>1.6595744680851066E-2</v>
       </c>
       <c r="J14" s="2">
-        <v>2.94</v>
+        <v>0.47</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="1"/>
-        <v>1.6851034561815786E-2</v>
+        <f>SUM(J14:J15)/J5</f>
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="2"/>
-        <v>0.19799965610133549</v>
+        <f t="shared" si="1"/>
+        <v>0.19387500000000002</v>
       </c>
     </row>
     <row r="15" spans="7:12" x14ac:dyDescent="0.3">
@@ -694,20 +698,321 @@
         <v>1.1744680851063831E-2</v>
       </c>
       <c r="J15" s="2">
-        <v>2.0499999999999998</v>
+        <v>1.18</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="1"/>
-        <v>1.1749871038000801E-2</v>
+        <f t="shared" ref="K15:K23" si="2">J15/$J$5</f>
+        <v>1.18E-2</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1380609846965094</v>
+        <f t="shared" si="1"/>
+        <v>0.13865</v>
       </c>
     </row>
     <row r="16" spans="7:12" x14ac:dyDescent="0.3">
       <c r="I16" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <v>80.599999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <v>0.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B938745-C031-44EB-8DE0-C90EAC00962D}">
+  <dimension ref="G4:L22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="3">
+        <f>J5-SUM(J7:J15)</f>
+        <v>78063</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1">
+        <f>4.371/2</f>
+        <v>2.1855000000000002</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" ref="I7:I14" si="0">H7/$I$5</f>
+        <v>0.21855000000000002</v>
+      </c>
+      <c r="J7" s="2">
+        <v>6490</v>
+      </c>
+      <c r="K7" s="1">
+        <f>SUM(J7:J15)/J5</f>
+        <v>0.21937000000000001</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" ref="L7:L15" si="1">K7*$I$5</f>
+        <v>2.1937000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1">
+        <f>3.095/2</f>
+        <v>1.5475000000000001</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.15475</v>
+      </c>
+      <c r="J8" s="2">
+        <v>4530</v>
+      </c>
+      <c r="K8" s="1">
+        <f>SUM(J8:J15)/J5</f>
+        <v>0.15447</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5447</v>
+      </c>
+    </row>
+    <row r="9" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f>2.19/2</f>
+        <v>1.095</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1095</v>
+      </c>
+      <c r="J9" s="2">
+        <v>3160</v>
+      </c>
+      <c r="K9" s="1">
+        <f>SUM(J9:J15)/J5</f>
+        <v>0.10917</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0917000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>-3</v>
+      </c>
+      <c r="H10" s="1">
+        <f>1.551/2</f>
+        <v>0.77549999999999997</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>7.7549999999999994E-2</v>
+      </c>
+      <c r="J10" s="2">
+        <v>2260</v>
+      </c>
+      <c r="K10" s="1">
+        <f>SUM(J10:J15)/J5</f>
+        <v>7.757E-2</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77570000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>-6</v>
+      </c>
+      <c r="H11">
+        <f>1.098/2</f>
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4900000000000004E-2</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1620</v>
+      </c>
+      <c r="K11" s="1">
+        <f>SUM(J11:J15)/J5</f>
+        <v>5.4969999999999998E-2</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.54969999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>-9</v>
+      </c>
+      <c r="H12" s="1">
+        <f>0.777/2</f>
+        <v>0.38850000000000001</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>3.8850000000000003E-2</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1130</v>
+      </c>
+      <c r="K12" s="1">
+        <f>SUM(J12:J15)/J5</f>
+        <v>3.8769999999999999E-2</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.38769999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>-12</v>
+      </c>
+      <c r="H13">
+        <f>0.55/2</f>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7500000000000004E-2</v>
+      </c>
+      <c r="J13" s="2">
+        <v>787</v>
+      </c>
+      <c r="K13" s="1">
+        <f>SUM(J13:J15)/J5</f>
+        <v>2.7470000000000001E-2</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.2747</v>
+      </c>
+    </row>
+    <row r="14" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>-18</v>
+      </c>
+      <c r="H14">
+        <f>0.39/2</f>
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.95E-2</v>
+      </c>
+      <c r="J14" s="2">
+        <v>560</v>
+      </c>
+      <c r="K14" s="1">
+        <f>SUM(J14:J15)/J5</f>
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.19600000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>-21</v>
+      </c>
+      <c r="H15">
+        <f>0.276/2</f>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="I15" s="1">
+        <f>H15/$I$5</f>
+        <v>1.3800000000000002E-2</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1400</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" ref="K15:K23" si="2">J15/$J$5</f>
+        <v>1.4E-2</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <v>76800</v>
+      </c>
+    </row>
+    <row r="21" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J21">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J22">
+        <f>J21+J20</f>
+        <v>78070</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated meters resistor values
</commit_message>
<xml_diff>
--- a/dBu meter calculation.xlsx
+++ b/dBu meter calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Documents\GitHub\DMH-Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CC431F-3169-44F1-9A9D-9FEEABB9083C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF86C738-54B7-479B-BF50-CA34E7C9B7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{34920A5C-097A-4EEA-8361-CAFEEE971C72}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
   <si>
     <t>dBu</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>total</t>
-  </si>
-  <si>
-    <t>TOTAL R (kOhms)</t>
   </si>
   <si>
     <t>TOTAL R (Ohms)</t>
@@ -113,11 +110,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62D02EB-515C-4A0B-BB92-62D83B04599D}">
-  <dimension ref="G4:L20"/>
+  <dimension ref="E4:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,7 +462,7 @@
     <col min="10" max="10" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="7:14" x14ac:dyDescent="0.3">
       <c r="I4" t="s">
         <v>3</v>
       </c>
@@ -472,15 +470,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="7:14" x14ac:dyDescent="0.3">
       <c r="I5">
-        <v>11.7</v>
+        <v>11.75</v>
       </c>
       <c r="J5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="7:12" x14ac:dyDescent="0.3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
         <v>0</v>
       </c>
@@ -491,13 +489,17 @@
         <v>2</v>
       </c>
       <c r="J6" s="3">
-        <f>J5-SUM(J7:J15)</f>
-        <v>81.349999999999994</v>
+        <v>82000</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="L6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G7">
         <v>6</v>
       </c>
@@ -507,21 +509,29 @@
       </c>
       <c r="I7" s="1">
         <f t="shared" ref="I7:I14" si="0">H7/$I$5</f>
-        <v>0.18679487179487184</v>
-      </c>
-      <c r="J7" s="2">
-        <v>5.49</v>
+        <v>0.18600000000000003</v>
+      </c>
+      <c r="J7" s="4">
+        <v>5600</v>
       </c>
       <c r="K7" s="1">
-        <f>SUM(J7:J15)/J5</f>
-        <v>0.1865</v>
+        <f>SUM(J7:J16)/J5</f>
+        <v>0.18840000000000001</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" ref="L7:L15" si="1">K7*$I$5</f>
-        <v>2.1820499999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="7:12" x14ac:dyDescent="0.3">
+        <v>2.2137000000000002</v>
+      </c>
+      <c r="M7" s="1">
+        <f>SUM(J7:J16)/SUM(J6:J16)</f>
+        <v>0.18683062276874257</v>
+      </c>
+      <c r="N7" s="1">
+        <f>M7*$I$5</f>
+        <v>2.1952598175327251</v>
+      </c>
+    </row>
+    <row r="8" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G8">
         <v>3</v>
       </c>
@@ -531,21 +541,29 @@
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>0.13226495726495729</v>
-      </c>
-      <c r="J8" s="2">
-        <v>3.83</v>
+        <v>0.13170212765957448</v>
+      </c>
+      <c r="J8" s="4">
+        <v>3900</v>
       </c>
       <c r="K8" s="1">
-        <f>SUM(J8:J15)/J5</f>
-        <v>0.13160000000000002</v>
+        <f>SUM(J8:J16)/J5</f>
+        <v>0.13239999999999999</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="1"/>
-        <v>1.5397200000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="7:12" x14ac:dyDescent="0.3">
+        <v>1.5556999999999999</v>
+      </c>
+      <c r="M8" s="1">
+        <f>SUM(J8:J16)/SUM(J6:J16)</f>
+        <v>0.13129710432368108</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" ref="N8:N16" si="2">M8*$I$5</f>
+        <v>1.5427409758032526</v>
+      </c>
+    </row>
+    <row r="9" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G9">
         <v>0</v>
       </c>
@@ -555,21 +573,29 @@
       </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>9.358974358974359E-2</v>
-      </c>
-      <c r="J9" s="2">
-        <v>2.74</v>
+        <v>9.3191489361702129E-2</v>
+      </c>
+      <c r="J9" s="4">
+        <v>2700</v>
       </c>
       <c r="K9" s="1">
-        <f>SUM(J9:J15)/J5</f>
-        <v>9.3299999999999994E-2</v>
+        <f>SUM(J9:J16)/J5</f>
+        <v>9.3399999999999997E-2</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="1"/>
-        <v>1.09161</v>
-      </c>
-    </row>
-    <row r="10" spans="7:12" x14ac:dyDescent="0.3">
+        <v>1.09745</v>
+      </c>
+      <c r="M9" s="1">
+        <f>SUM(J9:J16)/SUM(J6:J16)</f>
+        <v>9.2621975406584692E-2</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0883082110273701</v>
+      </c>
+    </row>
+    <row r="10" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G10">
         <v>-3</v>
       </c>
@@ -579,21 +605,29 @@
       </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>6.628205128205128E-2</v>
-      </c>
-      <c r="J10" s="2">
-        <v>1.91</v>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="J10" s="4">
+        <v>2000</v>
       </c>
       <c r="K10" s="1">
-        <f>SUM(J10:J15)/J5</f>
-        <v>6.5899999999999986E-2</v>
+        <f>SUM(J10:J16)/J5</f>
+        <v>6.6400000000000001E-2</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="1"/>
-        <v>0.77102999999999977</v>
-      </c>
-    </row>
-    <row r="11" spans="7:12" x14ac:dyDescent="0.3">
+        <v>0.7802</v>
+      </c>
+      <c r="M10" s="1">
+        <f>SUM(J10:J16)/SUM(J6:J16)</f>
+        <v>6.5846886156287185E-2</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="2"/>
+        <v>0.77370091233637439</v>
+      </c>
+    </row>
+    <row r="11" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G11">
         <v>-6</v>
       </c>
@@ -603,21 +637,29 @@
       </c>
       <c r="I11" s="1">
         <f t="shared" si="0"/>
-        <v>4.6923076923076928E-2</v>
-      </c>
-      <c r="J11" s="2">
-        <v>1.37</v>
+        <v>4.6723404255319151E-2</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1300</v>
       </c>
       <c r="K11" s="1">
-        <f>SUM(J11:J15)/J5</f>
-        <v>4.6799999999999994E-2</v>
+        <f>SUM(J11:J16)/J5</f>
+        <v>4.6399999999999997E-2</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="1"/>
-        <v>0.54755999999999994</v>
-      </c>
-    </row>
-    <row r="12" spans="7:12" x14ac:dyDescent="0.3">
+        <v>0.54519999999999991</v>
+      </c>
+      <c r="M11" s="1">
+        <f>SUM(J11:J16)/SUM(J6:J16)</f>
+        <v>4.6013486711622371E-2</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="2"/>
+        <v>0.54065846886156288</v>
+      </c>
+    </row>
+    <row r="12" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G12">
         <v>-9</v>
       </c>
@@ -627,21 +669,29 @@
       </c>
       <c r="I12" s="1">
         <f t="shared" si="0"/>
-        <v>3.3205128205128207E-2</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.98</v>
+        <v>3.3063829787234045E-2</v>
+      </c>
+      <c r="J12" s="4">
+        <v>1000</v>
       </c>
       <c r="K12" s="1">
-        <f>SUM(J12:J15)/J5</f>
-        <v>3.3099999999999997E-2</v>
+        <f>SUM(J12:J16)/J5</f>
+        <v>3.3399999999999999E-2</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" si="1"/>
-        <v>0.38726999999999995</v>
-      </c>
-    </row>
-    <row r="13" spans="7:12" x14ac:dyDescent="0.3">
+        <v>0.39244999999999997</v>
+      </c>
+      <c r="M12" s="1">
+        <f>SUM(J12:J16)/SUM(J6:J16)</f>
+        <v>3.3121777072590244E-2</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="2"/>
+        <v>0.38918088060293538</v>
+      </c>
+    </row>
+    <row r="13" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G13">
         <v>-12</v>
       </c>
@@ -651,21 +701,29 @@
       </c>
       <c r="I13" s="1">
         <f t="shared" si="0"/>
-        <v>2.3504273504273508E-2</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0.68</v>
+        <v>2.3404255319148939E-2</v>
+      </c>
+      <c r="J13" s="4">
+        <v>680</v>
       </c>
       <c r="K13" s="1">
-        <f>SUM(J13:J15)/J5</f>
-        <v>2.3300000000000001E-2</v>
+        <f>SUM(J13:J16)/J5</f>
+        <v>2.3400000000000001E-2</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" si="1"/>
-        <v>0.27261000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="7:12" x14ac:dyDescent="0.3">
+        <v>0.27495000000000003</v>
+      </c>
+      <c r="M13" s="1">
+        <f>SUM(J13:J16)/SUM(J6:J16)</f>
+        <v>2.3205077350257834E-2</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="2"/>
+        <v>0.27265965886552956</v>
+      </c>
+    </row>
+    <row r="14" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G14">
         <v>-15</v>
       </c>
@@ -675,21 +733,29 @@
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>1.666666666666667E-2</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0.47</v>
+        <v>1.6595744680851066E-2</v>
+      </c>
+      <c r="J14" s="4">
+        <v>510</v>
       </c>
       <c r="K14" s="1">
-        <f>SUM(J14:J15)/J5</f>
-        <v>1.6500000000000001E-2</v>
+        <f>SUM(J14:J16)/J5</f>
+        <v>1.66E-2</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="1"/>
-        <v>0.19305</v>
-      </c>
-    </row>
-    <row r="15" spans="7:12" x14ac:dyDescent="0.3">
+        <v>0.19505</v>
+      </c>
+      <c r="M14" s="1">
+        <f>SUM(J14:J16)/SUM(J6:J16)</f>
+        <v>1.6461721539071796E-2</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1934252280840936</v>
+      </c>
+    </row>
+    <row r="15" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G15">
         <v>-18</v>
       </c>
@@ -699,37 +765,62 @@
       </c>
       <c r="I15" s="1">
         <f>H15/$I$5</f>
-        <v>1.1794871794871797E-2</v>
-      </c>
-      <c r="J15" s="2">
-        <v>1.18</v>
+        <v>1.1744680851063831E-2</v>
+      </c>
+      <c r="J15" s="4">
+        <v>330</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" ref="K15" si="2">J15/$J$5</f>
-        <v>1.18E-2</v>
+        <f>SUM(J15:J16)/J6</f>
+        <v>1.4024390243902439E-2</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="1"/>
-        <v>0.13805999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="7:12" x14ac:dyDescent="0.3">
+        <v>0.16478658536585367</v>
+      </c>
+      <c r="M15" s="1">
+        <f>SUM(J15:J16)/SUM(J6:J16)</f>
+        <v>1.1404204680682269E-2</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="2"/>
+        <v>0.13399940499801666</v>
+      </c>
+    </row>
+    <row r="16" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G16">
         <v>-21</v>
       </c>
-      <c r="I16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J19">
-        <v>80.599999999999994</v>
-      </c>
-    </row>
-    <row r="20" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J20">
-        <v>0.75</v>
-      </c>
+      <c r="H16" s="1">
+        <f>0.195/2</f>
+        <v>9.7500000000000003E-2</v>
+      </c>
+      <c r="I16" s="1">
+        <f>H16/$I$5</f>
+        <v>8.2978723404255328E-3</v>
+      </c>
+      <c r="J16" s="4">
+        <v>820</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" ref="K16" si="3">J16/$J$5</f>
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" ref="L16" si="4">K16*$I$5</f>
+        <v>9.6350000000000005E-2</v>
+      </c>
+      <c r="M16" s="1">
+        <f>SUM(J16)/SUM(J6:J16)</f>
+        <v>8.1316937723125739E-3</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="2"/>
+        <v>9.5547401824672737E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -755,7 +846,7 @@
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="7:12" x14ac:dyDescent="0.3">
@@ -1029,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFC1236-186E-4F8D-ACF7-7671CAF785F5}">
-  <dimension ref="G4:L14"/>
+  <dimension ref="G4:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1046,7 +1137,7 @@
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="7:12" x14ac:dyDescent="0.3">
@@ -1054,7 +1145,8 @@
         <v>11.75</v>
       </c>
       <c r="J5">
-        <v>100000</v>
+        <f>SUM(J6:J9)</f>
+        <v>104500</v>
       </c>
     </row>
     <row r="6" spans="7:12" x14ac:dyDescent="0.3">
@@ -1068,13 +1160,17 @@
         <v>2</v>
       </c>
       <c r="J6" s="3">
-        <f>J5-SUM(J7:J9)</f>
-        <v>53130</v>
+        <v>56000</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="L6" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>14</v>
+      </c>
       <c r="H7" s="1">
         <v>5.5</v>
       </c>
@@ -1086,17 +1182,17 @@
         <v>8200</v>
       </c>
       <c r="K7" s="1">
-        <f>SUM(J7:J9)/J5</f>
-        <v>0.46870000000000001</v>
+        <f>SUM(J7:J9)/SUM(J6:J9)</f>
+        <v>0.46411483253588515</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" ref="L7:L9" si="1">K7*$I$5</f>
-        <v>5.507225</v>
+        <v>5.4533492822966503</v>
       </c>
     </row>
     <row r="8" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G8">
-        <v>11.25</v>
+        <v>12</v>
       </c>
       <c r="H8" s="1">
         <v>4.5</v>
@@ -1106,18 +1202,21 @@
         <v>0.38297872340425532</v>
       </c>
       <c r="J8" s="2">
-        <v>37400</v>
+        <v>39000</v>
       </c>
       <c r="K8" s="1">
-        <f>SUM(J8:J9)/$J$5</f>
-        <v>0.38669999999999999</v>
+        <f>SUM(J8:J9)/SUM(J6:J9)</f>
+        <v>0.38564593301435407</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="1"/>
-        <v>4.5437250000000002</v>
+        <v>4.5313397129186601</v>
       </c>
     </row>
     <row r="9" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>-17</v>
+      </c>
       <c r="H9" s="1">
         <f>0.15</f>
         <v>0.15</v>
@@ -1127,30 +1226,20 @@
         <v>1.276595744680851E-2</v>
       </c>
       <c r="J9" s="2">
-        <v>1270</v>
+        <v>1300</v>
       </c>
       <c r="K9" s="1">
-        <f>SUM(J9:J9)/$J$5</f>
-        <v>1.2699999999999999E-2</v>
+        <f>SUM(J9:J9)/SUM(J6:J9)</f>
+        <v>1.2440191387559809E-2</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="1"/>
-        <v>0.149225</v>
+        <v>0.14617224880382776</v>
       </c>
     </row>
     <row r="10" spans="7:12" x14ac:dyDescent="0.3">
       <c r="I10" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J13">
-        <v>52300</v>
-      </c>
-    </row>
-    <row r="14" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J14">
-        <v>820</v>
       </c>
     </row>
   </sheetData>

</xml_diff>